<commit_message>
edited to make work
</commit_message>
<xml_diff>
--- a/docs/DongleTemplate.xlsx
+++ b/docs/DongleTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesus\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50BBBCF-6A8E-44F7-B19C-D7FF8A3A5812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1326B7E1-8D28-43EE-88C2-30F16D95FFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="780" windowWidth="29040" windowHeight="15720" xr2:uid="{D5CD6C73-E1CB-4791-8588-61DEE1819B8A}"/>
   </bookViews>
@@ -666,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB611FD-7605-489B-A6C5-E445866AAA90}">
-  <dimension ref="C6:J76"/>
+  <dimension ref="C6:J108"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="N107" sqref="N107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1495,27 +1495,411 @@
       <c r="I74" s="16"/>
       <c r="J74" s="17"/>
     </row>
-    <row r="75" spans="3:10" ht="7.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C75" s="12"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="13"/>
-      <c r="F75" s="13"/>
-      <c r="G75" s="13"/>
-      <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="14"/>
-    </row>
-    <row r="76" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C76" s="9" t="s">
+    <row r="75" spans="3:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C75" s="15">
+        <v>65</v>
+      </c>
+      <c r="D75" s="16"/>
+      <c r="E75" s="16"/>
+      <c r="F75" s="16"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="16"/>
+      <c r="I75" s="16"/>
+      <c r="J75" s="17"/>
+    </row>
+    <row r="76" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C76" s="15">
+        <v>66</v>
+      </c>
+      <c r="D76" s="16"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="16"/>
+      <c r="G76" s="16"/>
+      <c r="H76" s="16"/>
+      <c r="I76" s="16"/>
+      <c r="J76" s="17"/>
+    </row>
+    <row r="77" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C77" s="15">
+        <v>67</v>
+      </c>
+      <c r="D77" s="16"/>
+      <c r="E77" s="16"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="16"/>
+      <c r="I77" s="16"/>
+      <c r="J77" s="17"/>
+    </row>
+    <row r="78" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C78" s="15">
+        <v>68</v>
+      </c>
+      <c r="D78" s="16"/>
+      <c r="E78" s="16"/>
+      <c r="F78" s="16"/>
+      <c r="G78" s="16"/>
+      <c r="H78" s="16"/>
+      <c r="I78" s="16"/>
+      <c r="J78" s="17"/>
+    </row>
+    <row r="79" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C79" s="15">
+        <v>69</v>
+      </c>
+      <c r="D79" s="16"/>
+      <c r="E79" s="16"/>
+      <c r="F79" s="16"/>
+      <c r="G79" s="16"/>
+      <c r="H79" s="16"/>
+      <c r="I79" s="16"/>
+      <c r="J79" s="17"/>
+    </row>
+    <row r="80" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C80" s="15">
+        <v>70</v>
+      </c>
+      <c r="D80" s="16"/>
+      <c r="E80" s="16"/>
+      <c r="F80" s="16"/>
+      <c r="G80" s="16"/>
+      <c r="H80" s="16"/>
+      <c r="I80" s="16"/>
+      <c r="J80" s="17"/>
+    </row>
+    <row r="81" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C81" s="15">
+        <v>71</v>
+      </c>
+      <c r="D81" s="16"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="16"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="16"/>
+      <c r="I81" s="16"/>
+      <c r="J81" s="17"/>
+    </row>
+    <row r="82" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C82" s="15">
+        <v>72</v>
+      </c>
+      <c r="D82" s="16"/>
+      <c r="E82" s="16"/>
+      <c r="F82" s="16"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="16"/>
+      <c r="I82" s="16"/>
+      <c r="J82" s="17"/>
+    </row>
+    <row r="83" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C83" s="15">
+        <v>73</v>
+      </c>
+      <c r="D83" s="16"/>
+      <c r="E83" s="16"/>
+      <c r="F83" s="16"/>
+      <c r="G83" s="16"/>
+      <c r="H83" s="16"/>
+      <c r="I83" s="16"/>
+      <c r="J83" s="17"/>
+    </row>
+    <row r="84" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C84" s="15">
+        <v>74</v>
+      </c>
+      <c r="D84" s="16"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="16"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="16"/>
+      <c r="I84" s="16"/>
+      <c r="J84" s="17"/>
+    </row>
+    <row r="85" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C85" s="15">
+        <v>75</v>
+      </c>
+      <c r="D85" s="16"/>
+      <c r="E85" s="16"/>
+      <c r="F85" s="16"/>
+      <c r="G85" s="16"/>
+      <c r="H85" s="16"/>
+      <c r="I85" s="16"/>
+      <c r="J85" s="17"/>
+    </row>
+    <row r="86" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C86" s="15">
+        <v>76</v>
+      </c>
+      <c r="D86" s="16"/>
+      <c r="E86" s="16"/>
+      <c r="F86" s="16"/>
+      <c r="G86" s="16"/>
+      <c r="H86" s="16"/>
+      <c r="I86" s="16"/>
+      <c r="J86" s="17"/>
+    </row>
+    <row r="87" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C87" s="15">
+        <v>77</v>
+      </c>
+      <c r="D87" s="16"/>
+      <c r="E87" s="16"/>
+      <c r="F87" s="16"/>
+      <c r="G87" s="16"/>
+      <c r="H87" s="16"/>
+      <c r="I87" s="16"/>
+      <c r="J87" s="17"/>
+    </row>
+    <row r="88" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C88" s="15">
+        <v>78</v>
+      </c>
+      <c r="D88" s="16"/>
+      <c r="E88" s="16"/>
+      <c r="F88" s="16"/>
+      <c r="G88" s="16"/>
+      <c r="H88" s="16"/>
+      <c r="I88" s="16"/>
+      <c r="J88" s="17"/>
+    </row>
+    <row r="89" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C89" s="15">
+        <v>79</v>
+      </c>
+      <c r="D89" s="16"/>
+      <c r="E89" s="16"/>
+      <c r="F89" s="16"/>
+      <c r="G89" s="16"/>
+      <c r="H89" s="16"/>
+      <c r="I89" s="16"/>
+      <c r="J89" s="17"/>
+    </row>
+    <row r="90" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C90" s="15">
+        <v>80</v>
+      </c>
+      <c r="D90" s="16"/>
+      <c r="E90" s="16"/>
+      <c r="F90" s="16"/>
+      <c r="G90" s="16"/>
+      <c r="H90" s="16"/>
+      <c r="I90" s="16"/>
+      <c r="J90" s="17"/>
+    </row>
+    <row r="91" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C91" s="15">
+        <v>81</v>
+      </c>
+      <c r="D91" s="16"/>
+      <c r="E91" s="16"/>
+      <c r="F91" s="16"/>
+      <c r="G91" s="16"/>
+      <c r="H91" s="16"/>
+      <c r="I91" s="16"/>
+      <c r="J91" s="17"/>
+    </row>
+    <row r="92" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C92" s="15">
+        <v>82</v>
+      </c>
+      <c r="D92" s="16"/>
+      <c r="E92" s="16"/>
+      <c r="F92" s="16"/>
+      <c r="G92" s="16"/>
+      <c r="H92" s="16"/>
+      <c r="I92" s="16"/>
+      <c r="J92" s="17"/>
+    </row>
+    <row r="93" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C93" s="15">
+        <v>83</v>
+      </c>
+      <c r="D93" s="16"/>
+      <c r="E93" s="16"/>
+      <c r="F93" s="16"/>
+      <c r="G93" s="16"/>
+      <c r="H93" s="16"/>
+      <c r="I93" s="16"/>
+      <c r="J93" s="17"/>
+    </row>
+    <row r="94" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C94" s="15">
+        <v>84</v>
+      </c>
+      <c r="D94" s="16"/>
+      <c r="E94" s="16"/>
+      <c r="F94" s="16"/>
+      <c r="G94" s="16"/>
+      <c r="H94" s="16"/>
+      <c r="I94" s="16"/>
+      <c r="J94" s="17"/>
+    </row>
+    <row r="95" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C95" s="15">
+        <v>85</v>
+      </c>
+      <c r="D95" s="16"/>
+      <c r="E95" s="16"/>
+      <c r="F95" s="16"/>
+      <c r="G95" s="16"/>
+      <c r="H95" s="16"/>
+      <c r="I95" s="16"/>
+      <c r="J95" s="17"/>
+    </row>
+    <row r="96" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C96" s="15">
+        <v>86</v>
+      </c>
+      <c r="D96" s="16"/>
+      <c r="E96" s="16"/>
+      <c r="F96" s="16"/>
+      <c r="G96" s="16"/>
+      <c r="H96" s="16"/>
+      <c r="I96" s="16"/>
+      <c r="J96" s="17"/>
+    </row>
+    <row r="97" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C97" s="15">
+        <v>87</v>
+      </c>
+      <c r="D97" s="16"/>
+      <c r="E97" s="16"/>
+      <c r="F97" s="16"/>
+      <c r="G97" s="16"/>
+      <c r="H97" s="16"/>
+      <c r="I97" s="16"/>
+      <c r="J97" s="17"/>
+    </row>
+    <row r="98" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C98" s="15">
+        <v>88</v>
+      </c>
+      <c r="D98" s="16"/>
+      <c r="E98" s="16"/>
+      <c r="F98" s="16"/>
+      <c r="G98" s="16"/>
+      <c r="H98" s="16"/>
+      <c r="I98" s="16"/>
+      <c r="J98" s="17"/>
+    </row>
+    <row r="99" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C99" s="15">
+        <v>89</v>
+      </c>
+      <c r="D99" s="16"/>
+      <c r="E99" s="16"/>
+      <c r="F99" s="16"/>
+      <c r="G99" s="16"/>
+      <c r="H99" s="16"/>
+      <c r="I99" s="16"/>
+      <c r="J99" s="17"/>
+    </row>
+    <row r="100" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C100" s="15">
+        <v>90</v>
+      </c>
+      <c r="D100" s="16"/>
+      <c r="E100" s="16"/>
+      <c r="F100" s="16"/>
+      <c r="G100" s="16"/>
+      <c r="H100" s="16"/>
+      <c r="I100" s="16"/>
+      <c r="J100" s="17"/>
+    </row>
+    <row r="101" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C101" s="15">
+        <v>91</v>
+      </c>
+      <c r="D101" s="16"/>
+      <c r="E101" s="16"/>
+      <c r="F101" s="16"/>
+      <c r="G101" s="16"/>
+      <c r="H101" s="16"/>
+      <c r="I101" s="16"/>
+      <c r="J101" s="17"/>
+    </row>
+    <row r="102" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C102" s="15">
+        <v>92</v>
+      </c>
+      <c r="D102" s="16"/>
+      <c r="E102" s="16"/>
+      <c r="F102" s="16"/>
+      <c r="G102" s="16"/>
+      <c r="H102" s="16"/>
+      <c r="I102" s="16"/>
+      <c r="J102" s="17"/>
+    </row>
+    <row r="103" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C103" s="15">
+        <v>93</v>
+      </c>
+      <c r="D103" s="16"/>
+      <c r="E103" s="16"/>
+      <c r="F103" s="16"/>
+      <c r="G103" s="16"/>
+      <c r="H103" s="16"/>
+      <c r="I103" s="16"/>
+      <c r="J103" s="17"/>
+    </row>
+    <row r="104" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C104" s="15">
+        <v>94</v>
+      </c>
+      <c r="D104" s="16"/>
+      <c r="E104" s="16"/>
+      <c r="F104" s="16"/>
+      <c r="G104" s="16"/>
+      <c r="H104" s="16"/>
+      <c r="I104" s="16"/>
+      <c r="J104" s="17"/>
+    </row>
+    <row r="105" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C105" s="15">
+        <v>95</v>
+      </c>
+      <c r="D105" s="16"/>
+      <c r="E105" s="16"/>
+      <c r="F105" s="16"/>
+      <c r="G105" s="16"/>
+      <c r="H105" s="16"/>
+      <c r="I105" s="16"/>
+      <c r="J105" s="17"/>
+    </row>
+    <row r="106" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C106" s="15">
+        <v>96</v>
+      </c>
+      <c r="D106" s="16"/>
+      <c r="E106" s="16"/>
+      <c r="F106" s="16"/>
+      <c r="G106" s="16"/>
+      <c r="H106" s="16"/>
+      <c r="I106" s="16"/>
+      <c r="J106" s="17"/>
+    </row>
+    <row r="107" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C107" s="12"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="13"/>
+      <c r="G107" s="13"/>
+      <c r="H107" s="13"/>
+      <c r="I107" s="13"/>
+      <c r="J107" s="14"/>
+    </row>
+    <row r="108" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C108" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D76" s="10"/>
-      <c r="E76" s="10"/>
-      <c r="F76" s="10"/>
-      <c r="G76" s="10"/>
-      <c r="H76" s="10"/>
-      <c r="I76" s="10"/>
-      <c r="J76" s="11"/>
+      <c r="D108" s="10"/>
+      <c r="E108" s="10"/>
+      <c r="F108" s="10"/>
+      <c r="G108" s="10"/>
+      <c r="H108" s="10"/>
+      <c r="I108" s="10"/>
+      <c r="J108" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>